<commit_message>
fix bug of chinese name
</commit_message>
<xml_diff>
--- a/clazzs.xlsx
+++ b/clazzs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\Java课堂代码\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\JavaLecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FA712C-A7FA-42E5-9693-3D52199BAA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397EB865-C86A-4595-91CD-1613B8BE600A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="163">
   <si>
     <t>20计网</t>
   </si>
@@ -519,6 +519,21 @@
   </si>
   <si>
     <t>晏仔强</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>错误名字去除字符列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>错误名字指定转化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(（?机电一体化[4四]?班～?）?)|(22级)|(机电22)|(机电[4四]?班?)</t>
+  </si>
+  <si>
+    <t>21电商[二2]?班?,</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -844,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -855,9 +870,11 @@
     <col min="1" max="2" width="15.08203125" customWidth="1"/>
     <col min="3" max="3" width="31.58203125" customWidth="1"/>
     <col min="4" max="4" width="34.25" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" customWidth="1"/>
+    <col min="6" max="6" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -870,8 +887,14 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -884,8 +907,11 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -895,8 +921,11 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -909,8 +938,11 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -922,6 +954,9 @@
       </c>
       <c r="D5" t="s">
         <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>